<commit_message>
Unmerged & Merged Cell Issue Fixed
</commit_message>
<xml_diff>
--- a/Excel/Mingguan/Excel/List Tugas Minggu Ke-2 (2 Agustus 2021 - 8 Agustus 2021).xlsx
+++ b/Excel/Mingguan/Excel/List Tugas Minggu Ke-2 (2 Agustus 2021 - 8 Agustus 2021).xlsx
@@ -1258,7 +1258,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I16" s="3" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="J16" s="8" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>